<commit_message>
updated ddqn config and checkpoint naming
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thodorischaros/Documents/MSc/AIDL_B02_AdvancedTopicsInDeepLearning/assignments/RL-Space-Invaders-DQN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCFF7DD-27A7-D84E-8376-E979080EF28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E2A936-A85E-BD46-AD45-E8746F0F933D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16800" xr2:uid="{236AF632-8DD9-4934-8E71-0C5E8EE714BF}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -605,10 +605,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="C4" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D4" s="2">
         <v>32</v>
@@ -617,7 +617,7 @@
         <v>1000000</v>
       </c>
       <c r="F4" s="2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G4" s="2">
         <v>150000</v>

</xml_diff>